<commit_message>
Feature: Deploy to Vercel
</commit_message>
<xml_diff>
--- a/data/flask_output_file.xlsx
+++ b/data/flask_output_file.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Real estate law is a branch of law that deals with the legal rights and duties of people who buy, sell, own, or lease land and buildings.</t>
+          <t>Real estate law refers to the laws and regulations that govern the ownership, lease, and use of real property. Real estate law generally covers issues such as title registration, zoning, and landlord-tenant rights.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Real estate law is different from other legal professions in a few ways. One way is that real estate law generally deals with the purchase, sale, and development of land and property, while other legal professions may deal with other areas of the law. Additionally, real estate law often requires specific knowledge of local zoning laws and regulations, which other legal professions may not require. Finally, real estate law may involve more contact with clients and potential clients than other legal professions, as real estate transactions often involve a significant amount of negotiation and face-to-face interaction.</t>
+          <t>Real estate law is different from other legal professions in a few ways. One way is that real estate law generally deals with physical property, whereas other legal professions may deal with intangible property, like copyrights or patents. Additionally, real estate law is usually geographically specific, meaning that lawyers need to be familiar with the laws of the jurisdiction in which they practice. Finally, real estate law often involves complex transactions, and lawyers must be able to navigate these transactions in order to protect their clients' interests.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Most real estate lawyers do a variety of work for clients, such as helping them purchase property, preparing and reviewing purchase contracts, assisting with mortgages and other financing, overseeing real estate closings, and handling evictions and other landlord-tenant disputes. Some real estate lawyers also handle zoning issues and litigation, such as eminent domain cases.</t>
+          <t>The answer may vary depending on which country you are asking about, but in general, real estate lawyers are involved in any legal issues related to real estate, such as buying, selling, leasing, and zoning.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>The legal profession can be extremely competitive, and specialization can be one way to set yourself apart from other lawyers. Real estate law is a specialized area of law that deals with the sale, purchase, ownership, and use of real property. Because real estate transactions can be complex, a lawyer who specializes in real estate law can help their clients navigate the legal process and ensure that their rights are protected.</t>
+          <t>There are many aspects to real estate law. By specializing in this area, attorneys can become experts in the field and provide more comprehensive and clients. Additionally, real estate law is a complex and ever-changing area of the law, so specializing in this field can help attorneys stay abreast of the latest changes and developments.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>All types of legal transcription are useful in real estate law. This includes dictation of letters, memos, court proceedings, and client meetings.</t>
+          <t>There are a number of different types of real estate law transcription that can be useful, including contract law, property law, and title law. Transcription can also be useful for other aspects of real estate law, such as zoning law and environmental law.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>There are many ways that transcription can be used in real estate law. For example, transcription can be used to create a record of conversations between parties involved in a real estate transaction, such as the buyer, seller, broker, and loan officer. Transcription can also be used to create a record of inspections of a property, or to create a record of meetings between parties involved in a real estate dispute.</t>
+          <t>There are various ways in which real estate lawyers can utilize transcription. For instance, lawyers can use transcription to create a record of all the key points that are discussed during a real estate transaction. This can be extremely useful for lawyers who need to review the details of a transaction at a later date. Additionally, transcription can also be used to create a record of all the documents that are signed during a real estate transaction. This can be useful for lawyers who need to review the documents at a later date.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
@@ -762,15 +762,14 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>Real estate law is a branch of law that deals with the legal rights and duties of people who buy, sell, own, or lease land and buildings. Real estate law is different from other legal professions in a few ways. One way is that real estate law generally deals with the purchase, sale, and development of land and property, while other legal professions may deal with other areas of the law. Additionally, real estate law often requires specific knowledge of local zoning laws and regulations, which other legal professions may not require. Finally, real estate law may involve more contact with clients and potential clients than other legal professions, as real estate transactions often involve a significant amount of negotiation and face-to-face interaction. Most real estate lawyers do a variety of work for clients, such as helping them purchase property, preparing and reviewing purchase contracts, assisting with mortgages and other financing, overseeing real estate closings, and handling evictions and other landlord-tenant disputes. Some real estate lawyers also handle zoning issues and litigation, such as eminent domain cases. The legal profession can be extremely competitive, and specialization can be one way to set yourself apart from other lawyers. Real estate law is a specialized area of law that deals with the sale, purchase, ownership, and use of real property. Because real estate transactions can be complex, a lawyer who specializes in real estate law can help their clients navigate the legal process and ensure that their rights are protected. All types of legal transcription are useful in real estate law. This includes dictation of letters, memos, court proceedings, and client meetings. There are many ways that transcription can be used in real estate law. For example, transcription can be used to create a record of conversations between parties involved in a real estate transaction, such as the buyer, seller, broker, and loan officer. Transcription can also be used to create a record of inspections of a property, or to create a record of meetings between parties involved in a real estate dispute.</t>
+          <t>Real estate law refers to the laws and regulations that govern the ownership, lease, and use of real property. Real estate law generally covers issues such as title registration, zoning, and landlord-tenant rights. Real estate law is different from other legal professions in a few ways. One way is that real estate law generally deals with physical property, whereas other legal professions may deal with intangible property, like copyrights or patents. Additionally, real estate law is usually geographically specific, meaning that lawyers need to be familiar with the laws of the jurisdiction in which they practice. Finally, real estate law often involves complex transactions, and lawyers must be able to navigate these transactions in order to protect their clients' interests. The answer may vary depending on which country you are asking about, but in general, real estate lawyers are involved in any legal issues related to real estate, such as buying, selling, leasing, and zoning. There are many aspects to real estate law. By specializing in this area, attorneys can become experts in the field and provide more comprehensive and clients. Additionally, real estate law is a complex and ever-changing area of the law, so specializing in this field can help attorneys stay abreast of the latest changes and developments. There are a number of different types of real estate law transcription that can be useful, including contract law, property law, and title law. Transcription can also be useful for other aspects of real estate law, such as zoning law and environmental law. There are various ways in which real estate lawyers can utilize transcription. For instance, lawyers can use transcription to create a record of all the key points that are discussed during a real estate transaction. This can be extremely useful for lawyers who need to review the details of a transaction at a later date. Additionally, transcription can also be used to create a record of all the documents that are signed during a real estate transaction. This can be useful for lawyers who need to review the documents at a later date.</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>Real estate lawyers deal with complex transactions and legal processes, so having reliable transcription services can be invaluable. Capital Typing provides legal transcription services specifically for real estate attorneys. With our services, real estate attorneys can have all their conversations, letters, memos, court proceedings, and client meetings transcribed accurately and efficiently. 
-Legal transcription is an important part of real estate law. It allows lawyers to have a record of conversations between parties involved in a real estate transaction, as well as inspections of a property and meetings between parties involved in a real estate dispute. With Capital Typing's services, attorneys can have all of this information transcribed accurately and quickly.
-We understand the importance of accuracy and confidentiality in the real estate field. That's why all of our transcriptionists are experienced and knowledgeable in real estate law, so they can accurately transcribe conversations and documents. We also have strict privacy and security protocols in place, so your information is always kept secure. 
-At Capital</t>
+          <t>Real estate law is an important and complex field that requires lawyers to understand the laws in the jurisdiction in which they practice. With such an intricate and ever-changing area of the law, it’s essential for real estate lawyers to stay abreast of the latest changes and developments. For this reason, real estate lawyers can benefit greatly from legal transcription services.
+Legal transcription services are useful for a number of real estate law-related tasks. For instance, transcription can be used to create a record of all the documents that are signed during a real estate transaction. This can help lawyers review and keep track of the details of a transaction at a later date. Additionally, lawyers can use transcription to create a record of all the key points that are discussed during a real estate transaction. This can be useful for lawyers who need to review the details of a transaction at a later date.
+Furthermore, legal transcription services can also be used for other aspects of real estate law, such</t>
         </is>
       </c>
     </row>
@@ -782,7 +781,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A court reporter is a legal professional who uses two-way shorthand to create a word-for-word transcript of courtroom proceedings. Court reporters also work in other settings, such as business meetings and conferences, to create transcripts of the proceedings.</t>
+          <t>A court reporter is an individual who records and transcribes court proceedings. Court reporters use a special type of shorthand to take down verbatim transcripts of what is said in court. These transcripts can be used as evidence in legal proceedings.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -792,7 +791,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>While other legal professionals may work in courtrooms, court reporters are the only professionals who create transcripts of court proceedings. Court reporters use a stenograph machine, which uses a system of keys to record spoken words, to create a verbatim record of proceedings.</t>
+          <t>A court reporter is a legal professional who specializes in creating transcripts of court proceedings. Other legal professionals, such as lawyers and judges, may rely on court reporters to create accurate records of what was said during a court case.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -802,7 +801,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Court reporters can utilize legal transcription services in order to have their court proceedings transcribed into written form. This can be helpful in a number of ways, including creating a written record of the proceedings, making it easier to review the transcript later on, and providing a written transcript to parties who were not able to attend the court proceedings.</t>
+          <t>There are a number of ways that court reporters can utilize legal transcription services. First, court reporters can use transcription services to create transcripts of court proceedings. This can be useful for creating a record of what was said during a court case, or for creating a transcript for appeal purposes. Additionally, court reporters can use transcription services to create transcripts of depositions. This can be helpful for creating a record of what was said during a deposition, or for creating a transcript for use in future court proceedings.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -852,14 +851,14 @@
       </c>
       <c r="AR3" t="inlineStr">
         <is>
-          <t>A court reporter is a legal professional who uses two-way shorthand to create a word-for-word transcript of courtroom proceedings. Court reporters also work in other settings, such as business meetings and conferences, to create transcripts of the proceedings. While other legal professionals may work in courtrooms, court reporters are the only professionals who create transcripts of court proceedings. Court reporters use a stenograph machine, which uses a system of keys to record spoken words, to create a verbatim record of proceedings. Court reporters can utilize legal transcription services in order to have their court proceedings transcribed into written form. This can be helpful in a number of ways, including creating a written record of the proceedings, making it easier to review the transcript later on, and providing a written transcript to parties who were not able to attend the court proceedings.</t>
+          <t>A court reporter is an individual who records and transcribes court proceedings. Court reporters use a special type of shorthand to take down verbatim transcripts of what is said in court. These transcripts can be used as evidence in legal proceedings. A court reporter is a legal professional who specializes in creating transcripts of court proceedings. Other legal professionals, such as lawyers and judges, may rely on court reporters to create accurate records of what was said during a court case. There are a number of ways that court reporters can utilize legal transcription services. First, court reporters can use transcription services to create transcripts of court proceedings. This can be useful for creating a record of what was said during a court case, or for creating a transcript for appeal purposes. Additionally, court reporters can use transcription services to create transcripts of depositions. This can be helpful for creating a record of what was said during a deposition, or for creating a transcript for use in future court proceedings.</t>
         </is>
       </c>
       <c r="AS3" t="inlineStr">
         <is>
-          <t>Legal transcription services are an invaluable tool for court reporters and other legal professionals. Court reporters are the only legal professionals who use two-way shorthand to create a word-for-word transcript of courtroom proceedings. However, court reporters are also often called upon to create transcripts of proceedings in other settings such as business meetings and conferences. In order to do so, they use a stenograph machine, which employs a system of keys to record spoken words, to create a verbatim record of the proceedings.
-For court reporters, legal transcription services can be extremely beneficial. Having your court proceedings transcribed into written form can help in a variety of ways. First and foremost, it creates an easily accessible written record of the proceedings which can be accessed later on for review. Additionally, it can also provide a written transcript to parties who were unable to attend the court proceedings.
-Capital Typing provides comprehensive legal transcription services for court reporters. We understand the importance of accuracy and detail in court</t>
+          <t>Legal transcription services can be a valuable resource for court reporters. Court reporters are legal professionals who specialize in creating transcripts of court proceedings. They use a special type of shorthand to take down verbatim transcripts of what is said in court, which can be used as evidence in legal proceedings. Transcription services can provide court reporters with an efficient and accurate way to transcribe court proceedings and depositions.
+At Capital Typing, we provide legal transcription services for court reporters. Our services are designed to help court reporters create accurate records of court proceedings and depositions. We utilize the latest technology and experienced transcriptionists to ensure that your transcripts are accurate and of the highest quality.
+Our transcription services are tailored to the specific needs of court reporters. We can provide you with transcripts of court proceedings and depositions quickly and efficiently. Our experienced transcriptionists can transcribe in a variety of legal formats, including audio, video, and handwritten documents. We can also produce transcripts in a variety</t>
         </is>
       </c>
     </row>
@@ -871,12 +870,8 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Services to Your Company
-There are many reasons why a company decides to outsource its transcription. However, the overall main goal is to save on costs. With an expertise team in transcription, you can be assured quality with the least amount of time and effort out of your employees. The flexibility of our team can enable you to keep up with your business goals while leaving all transcription needs to us.
-We Offer Various Types of Transcription Services for Businesses
-Transcription is an important service that companies provide. Finest Typists Transcription services allow businesses to produce quality documents that can be legally binding. We offer all types of transcription service style that businesses require. Here is a table with all the services that we currently provide.
-Type Level of Accuracy Transcription Services Type I High Rate Medication Administration Operations type II Medium Rate Courtroom and Teleconference type III Low Rate Students’ note and Group discussio
-Does Your Business Need Transcription Services?</t>
+          <t>Services by Smart Transcribe
+As a freelance transcriptionist, I find dealing with multiple projects and clients quite a stressful task. Smart Transcribe have been extremely helpful in reducing this stress within my job. While they are always quick to respond to any of my requests, I have also found that they are extremely good at matching me to transcriptions that are within my range of abilities. As a result, I am very happy with the work that I have done for Smart Transcribe and the relationships I have formed with the company.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -886,8 +881,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>to market-leader Martech Cube for your content marketing efforts, podcasts, webinars and tutorials.
- steadman</t>
+          <t>There are quite a few reasons why some businesses choose to outsource transcription services. The savings in terms of both time and money is significant. Here we will explore some of the many benefits of outsourcing transcription services.
+The benefit of savings in terms of time is that businesses can redirect their energies to other tasks that invaluable. The time savings can really add up and help a business to get back on track.
+Another huge benefit of outsourcing transcription services is the reduction in turnover rates. With the increased accuracy that transcription services provide, businesses can keep better track of their turnover rates. This means that businesses can make more money and keep their customers happy.
+Transcription services can provide a wide variety of benefits. These benefits can be discovered by exploring the different types of services that outsourcing provides. With the increased accuracy that outsourcing provides, businesses can get back on track and improve their bottom line.
+Outsourcing can save businesses time and money and help to improve the overall quality</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -898,19 +896,9 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>Services
-Short-Term Tech Fixes Won't Fix the Nursing Shortage | Staffing Industry Analysts
-golden-standard-2019- Enablement, border2 point, AR
-Get Best Audio Transcription Services
-Banner Document Management
-langTrans Demo CD
-datascientists4health
-Best Medical Transcription Services
-Index of /wp-content/uploads/2016/07 .
-We Achieve 99.99% Accuracy!
-Open Briefing: Dry run: gamifying transparency to test interesting nuggets from intelligence reports
-Next time you would like a quote of accurate transcription services at the lowest price per minute, give me a call at 1 (877) 363 7399 or email me Harish ...
-Voicing's an essential part of your performance.
-Our high audio transcriptions are the state of art as well as it has been reviewed by technological expert for leave no error to protect your documents ...</t>
+A recent survey has found that the larger majority of employees working in corporate circles have a preference for working for companies that outsource transcription services. This means that companies are very interested in maintaining a successful image in the eyes of their employees. Therefore, compared to other companies that still hold onto their internalized transcription services, those that outsource transcription services are considered a better bet for career advancement.
+As a fertilizer for career growth, corporate transcription services are very useful. A recent study showed that compelling speech at conferences is two to three times more effective at getting ideas across than written messages. This means that corporate transcription services can help increase knowledge retention and boost effective communication in the workplace. Since successful communication is primary to effective learning, the impact of corporate transcription services is evident.
+Written transcription services have specific purposes and benefits. TheyLondon Private investigators can be used to record business meetings, transcribe speeches and yearly reports, and transcribe lectures. The availability of transcription services will make</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -921,7 +909,16 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>Services
-Any business looking to outsource transcription services, whether it be legal transcription services or medical transcription services, wants to know what measures are in place to protect their data security and confidentiality. There are a variety of ways that your transcription company can protect your data, including:</t>
+When you outsource transcription services to a third-party provider, you are relying on that provider to keep your information confidential. The transcription services company should have implementing security measures to protect your confidential information. The security measures might include the following:
+All employees are required to sign confidentiality agreements.
+All employees undergo criminal background checks prior to being hired.
+All employees are trained to handle and protect confidential information.
+Security as an employee is allowed access to a specific transcription services job.
+Recorded phone calls/conversations are protected per confidentiality agreement.
+Paper copies of transcripts are transmitted using physical securityring mail only.
+Auditing procedures in place to help ensure data security.
+Data management procedures and secure document sharing when you outsource transcription services.
+Transcription services companies use secure file sharing/transmission services and have strict rules about how files are to be transmitted (two-factor authentication, encryption, etc.).</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -969,34 +966,33 @@
       </c>
       <c r="AR4" t="inlineStr">
         <is>
-          <t>Services to Your Company
-There are many reasons why a company decides to outsource its transcription. However, the overall main goal is to save on costs. With an expertise team in transcription, you can be assured quality with the least amount of time and effort out of your employees. The flexibility of our team can enable you to keep up with your business goals while leaving all transcription needs to us.
-We Offer Various Types of Transcription Services for Businesses
-Transcription is an important service that companies provide. Finest Typists Transcription services allow businesses to produce quality documents that can be legally binding. We offer all types of transcription service style that businesses require. Here is a table with all the services that we currently provide.
-Type Level of Accuracy Transcription Services Type I High Rate Medication Administration Operations type II Medium Rate Courtroom and Teleconference type III Low Rate Students’ note and Group discussio
-Does Your Business Need Transcription Services? to market-leader Martech Cube for your content marketing efforts, podcasts, webinars and tutorials.
- steadman Services
-Short-Term Tech Fixes Won't Fix the Nursing Shortage | Staffing Industry Analysts
-golden-standard-2019- Enablement, border2 point, AR
-Get Best Audio Transcription Services
-Banner Document Management
-langTrans Demo CD
-datascientists4health
-Best Medical Transcription Services
-Index of /wp-content/uploads/2016/07 .
-We Achieve 99.99% Accuracy!
-Open Briefing: Dry run: gamifying transparency to test interesting nuggets from intelligence reports
-Next time you would like a quote of accurate transcription services at the lowest price per minute, give me a call at 1 (877) 363 7399 or email me Harish ...
-Voicing's an essential part of your performance.
-Our high audio transcriptions are the state of art as well as it has been reviewed by technological expert for leave no error to protect your documents ... Services
-Any business looking to outsource transcription services, whether it be legal transcription services or medical transcription services, wants to know what measures are in place to protect their data security and confidentiality. There are a variety of ways that your transcription company can protect your data, including:</t>
+          <t>Services by Smart Transcribe
+As a freelance transcriptionist, I find dealing with multiple projects and clients quite a stressful task. Smart Transcribe have been extremely helpful in reducing this stress within my job. While they are always quick to respond to any of my requests, I have also found that they are extremely good at matching me to transcriptions that are within my range of abilities. As a result, I am very happy with the work that I have done for Smart Transcribe and the relationships I have formed with the company. There are quite a few reasons why some businesses choose to outsource transcription services. The savings in terms of both time and money is significant. Here we will explore some of the many benefits of outsourcing transcription services.
+The benefit of savings in terms of time is that businesses can redirect their energies to other tasks that invaluable. The time savings can really add up and help a business to get back on track.
+Another huge benefit of outsourcing transcription services is the reduction in turnover rates. With the increased accuracy that transcription services provide, businesses can keep better track of their turnover rates. This means that businesses can make more money and keep their customers happy.
+Transcription services can provide a wide variety of benefits. These benefits can be discovered by exploring the different types of services that outsourcing provides. With the increased accuracy that outsourcing provides, businesses can get back on track and improve their bottom line.
+Outsourcing can save businesses time and money and help to improve the overall quality Services
+A recent survey has found that the larger majority of employees working in corporate circles have a preference for working for companies that outsource transcription services. This means that companies are very interested in maintaining a successful image in the eyes of their employees. Therefore, compared to other companies that still hold onto their internalized transcription services, those that outsource transcription services are considered a better bet for career advancement.
+As a fertilizer for career growth, corporate transcription services are very useful. A recent study showed that compelling speech at conferences is two to three times more effective at getting ideas across than written messages. This means that corporate transcription services can help increase knowledge retention and boost effective communication in the workplace. Since successful communication is primary to effective learning, the impact of corporate transcription services is evident.
+Written transcription services have specific purposes and benefits. TheyLondon Private investigators can be used to record business meetings, transcribe speeches and yearly reports, and transcribe lectures. The availability of transcription services will make Services
+When you outsource transcription services to a third-party provider, you are relying on that provider to keep your information confidential. The transcription services company should have implementing security measures to protect your confidential information. The security measures might include the following:
+All employees are required to sign confidentiality agreements.
+All employees undergo criminal background checks prior to being hired.
+All employees are trained to handle and protect confidential information.
+Security as an employee is allowed access to a specific transcription services job.
+Recorded phone calls/conversations are protected per confidentiality agreement.
+Paper copies of transcripts are transmitted using physical securityring mail only.
+Auditing procedures in place to help ensure data security.
+Data management procedures and secure document sharing when you outsource transcription services.
+Transcription services companies use secure file sharing/transmission services and have strict rules about how files are to be transmitted (two-factor authentication, encryption, etc.).</t>
         </is>
       </c>
       <c r="AS4" t="inlineStr">
         <is>
-          <t>For any business looking to outsource transcription services, there are a few key things they need to consider. First and foremost, they need to ensure that the transcription company they are using can guarantee the security and confidentiality of their data. This is essential as any information which is shared with the transcription company should remain secure and confidential.
-To ensure that data security and confidentiality are maintained, transcription companies can employ a variety of measures. These can include encrypting data, limiting access to data, and providing contractual agreements that ensure data is not shared with any other parties. Additionally, transcription companies should have protocols in place which allow for the secure storage and retrieval of data, as well as procedures for the secure destruction of data once it is no longer needed.
-The transcription company should also provide accurate and timely transcription services, as this is key to ensuring the business is able to meet its goals. At Finest Typists Transcription, we offer various types of transcription services, ranging from high</t>
+          <t>Businesses have found that outsourcing transcription services can save them both time and money. In addition to saving money, transcription services help to reduce turnover rates and promote better communication in the workplace. When done properly, outsourcing transcription services can provide a variety of benefits.
+One of the biggest benefits of outsourcing transcription services is the time savings that it can provide. When businesses outsource transcription services, they can redirect their energies to other tasks that are invaluable. This time savings can really add up and help a business to get back on track.
+Another benefit of outsourcing transcription services is the reduction in turnover rates. With the increased accuracy that transcription services provide, businesses can keep better track of their turnover rates. This means that businesses can make more money and keep their customers happy.
+In addition to the financial benefits that transcription services can provide, they can also help to improve the overall quality of communication in the workplace. A recent survey has found that the larger majority of employees working in corporate</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
BugFix: File Download Error
modified the URL to the output file
</commit_message>
<xml_diff>
--- a/data/flask_output_file.xlsx
+++ b/data/flask_output_file.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Real estate law refers to the laws and regulations that govern the ownership, lease, and use of real property. Real estate law generally covers issues such as title registration, zoning, and landlord-tenant rights.</t>
+          <t>Real estate law is a branch of civil law that covers the right to possess, use, and enjoy land and the permanent man-made additions attached to it.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Real estate law is different from other legal professions in a few ways. One way is that real estate law generally deals with physical property, whereas other legal professions may deal with intangible property, like copyrights or patents. Additionally, real estate law is usually geographically specific, meaning that lawyers need to be familiar with the laws of the jurisdiction in which they practice. Finally, real estate law often involves complex transactions, and lawyers must be able to navigate these transactions in order to protect their clients' interests.</t>
+          <t>Most real estate law is state law, which means that real estate lawyers must know the law of the state in which they practice. In addition, real estate lawyers must know about title insurance, zoning, and environmental law.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The answer may vary depending on which country you are asking about, but in general, real estate lawyers are involved in any legal issues related to real estate, such as buying, selling, leasing, and zoning.</t>
+          <t>A real estate lawyer is a type of lawyer who specializes in real estate law. Real estate lawyers help their clients with a variety of legal issues that relate to real estate, such as buying or selling property, landlord-tenant disputes, and property ownership disputes.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>There are many aspects to real estate law. By specializing in this area, attorneys can become experts in the field and provide more comprehensive and clients. Additionally, real estate law is a complex and ever-changing area of the law, so specializing in this field can help attorneys stay abreast of the latest changes and developments.</t>
+          <t>Real estate law is helpful in the legal profession because it deals with a specific area of law. This area of law deals with the buying, selling, and leasing of property.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -708,7 +708,16 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>There are a number of different types of real estate law transcription that can be useful, including contract law, property law, and title law. Transcription can also be useful for other aspects of real estate law, such as zoning law and environmental law.</t>
+          <t>The legal transcription of real estate law can be useful for a number of different areas, including:
+-Property law
+-Landlord-tenant law
+-Real estate contracts
+-Mortgages
+-Deeds
+-Leases
+-Evictions
+-Foreclosures
+-Zoning</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -718,7 +727,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>There are various ways in which real estate lawyers can utilize transcription. For instance, lawyers can use transcription to create a record of all the key points that are discussed during a real estate transaction. This can be extremely useful for lawyers who need to review the details of a transaction at a later date. Additionally, transcription can also be used to create a record of all the documents that are signed during a real estate transaction. This can be useful for lawyers who need to review the documents at a later date.</t>
+          <t>There are many ways that real estate lawyers can utilize transcription. One way is to use it to create transcripts of important meetings, such as offer meetings, agent meetings, or escrow meetings. This can provide a written record of what was said during the meeting, which can be useful for reference or for creating minutes. Another way that real estate lawyers can use transcription is to create transcripts of property inspections. This can be helpful for documenting the condition of the property and any repairs that need to be made.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
@@ -762,14 +771,23 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>Real estate law refers to the laws and regulations that govern the ownership, lease, and use of real property. Real estate law generally covers issues such as title registration, zoning, and landlord-tenant rights. Real estate law is different from other legal professions in a few ways. One way is that real estate law generally deals with physical property, whereas other legal professions may deal with intangible property, like copyrights or patents. Additionally, real estate law is usually geographically specific, meaning that lawyers need to be familiar with the laws of the jurisdiction in which they practice. Finally, real estate law often involves complex transactions, and lawyers must be able to navigate these transactions in order to protect their clients' interests. The answer may vary depending on which country you are asking about, but in general, real estate lawyers are involved in any legal issues related to real estate, such as buying, selling, leasing, and zoning. There are many aspects to real estate law. By specializing in this area, attorneys can become experts in the field and provide more comprehensive and clients. Additionally, real estate law is a complex and ever-changing area of the law, so specializing in this field can help attorneys stay abreast of the latest changes and developments. There are a number of different types of real estate law transcription that can be useful, including contract law, property law, and title law. Transcription can also be useful for other aspects of real estate law, such as zoning law and environmental law. There are various ways in which real estate lawyers can utilize transcription. For instance, lawyers can use transcription to create a record of all the key points that are discussed during a real estate transaction. This can be extremely useful for lawyers who need to review the details of a transaction at a later date. Additionally, transcription can also be used to create a record of all the documents that are signed during a real estate transaction. This can be useful for lawyers who need to review the documents at a later date.</t>
+          <t>Real estate law is a branch of civil law that covers the right to possess, use, and enjoy land and the permanent man-made additions attached to it. Most real estate law is state law, which means that real estate lawyers must know the law of the state in which they practice. In addition, real estate lawyers must know about title insurance, zoning, and environmental law. A real estate lawyer is a type of lawyer who specializes in real estate law. Real estate lawyers help their clients with a variety of legal issues that relate to real estate, such as buying or selling property, landlord-tenant disputes, and property ownership disputes. Real estate law is helpful in the legal profession because it deals with a specific area of law. This area of law deals with the buying, selling, and leasing of property. The legal transcription of real estate law can be useful for a number of different areas, including:
+-Property law
+-Landlord-tenant law
+-Real estate contracts
+-Mortgages
+-Deeds
+-Leases
+-Evictions
+-Foreclosures
+-Zoning There are many ways that real estate lawyers can utilize transcription. One way is to use it to create transcripts of important meetings, such as offer meetings, agent meetings, or escrow meetings. This can provide a written record of what was said during the meeting, which can be useful for reference or for creating minutes. Another way that real estate lawyers can use transcription is to create transcripts of property inspections. This can be helpful for documenting the condition of the property and any repairs that need to be made.</t>
         </is>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
-          <t>Real estate law is an important and complex field that requires lawyers to understand the laws in the jurisdiction in which they practice. With such an intricate and ever-changing area of the law, it’s essential for real estate lawyers to stay abreast of the latest changes and developments. For this reason, real estate lawyers can benefit greatly from legal transcription services.
-Legal transcription services are useful for a number of real estate law-related tasks. For instance, transcription can be used to create a record of all the documents that are signed during a real estate transaction. This can help lawyers review and keep track of the details of a transaction at a later date. Additionally, lawyers can use transcription to create a record of all the key points that are discussed during a real estate transaction. This can be useful for lawyers who need to review the details of a transaction at a later date.
-Furthermore, legal transcription services can also be used for other aspects of real estate law, such</t>
+          <t>Real estate law is a complex field of law that encompasses the rights to possess, use, and enjoy land and the permanent man-made structures attached to it. Since real estate law is largely governed by state law, real estate lawyers must be knowledgeable of the specific laws of the state in which they practice. In addition, real estate lawyers must understand title insurance, zoning, and environmental law.
+If you are a real estate lawyer, you may find legal transcription services to be a valuable tool in your practice. Legal transcription services can help you to create transcripts of important meetings, such as offer meetings, agent meetings, or escrow meetings. This can provide a written record of the conversations that took place during the meeting, which can be useful for reference or for creating minutes. Additionally, legal transcription can be used to create transcripts of property inspections, which can be helpful for documenting the condition of the property and any repairs that need to be made. 
+At Capital Typing,</t>
         </is>
       </c>
     </row>
@@ -781,7 +799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A court reporter is an individual who records and transcribes court proceedings. Court reporters use a special type of shorthand to take down verbatim transcripts of what is said in court. These transcripts can be used as evidence in legal proceedings.</t>
+          <t>A court reporter is an official who uses shorthand or other methods to transcribe judicial proceedings.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -791,7 +809,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>A court reporter is a legal professional who specializes in creating transcripts of court proceedings. Other legal professionals, such as lawyers and judges, may rely on court reporters to create accurate records of what was said during a court case.</t>
+          <t>A court reporter is different from other legal professionals because they are specifically trained to take down verbatim transcriptions of court proceedings. This means that they have to be able to type extremely quickly and accurately in order to keep up with the proceedings. Court reporters also often have to be able to create audio or video recordings of proceedings in addition to taking down the transcripts.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -801,7 +819,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>There are a number of ways that court reporters can utilize legal transcription services. First, court reporters can use transcription services to create transcripts of court proceedings. This can be useful for creating a record of what was said during a court case, or for creating a transcript for appeal purposes. Additionally, court reporters can use transcription services to create transcripts of depositions. This can be helpful for creating a record of what was said during a deposition, or for creating a transcript for use in future court proceedings.</t>
+          <t>There are many ways that court reporters can utilize legal transcription services. They can use them to transcribe witness testimony, court proceedings, and deposition transcripts.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -851,14 +869,15 @@
       </c>
       <c r="AR3" t="inlineStr">
         <is>
-          <t>A court reporter is an individual who records and transcribes court proceedings. Court reporters use a special type of shorthand to take down verbatim transcripts of what is said in court. These transcripts can be used as evidence in legal proceedings. A court reporter is a legal professional who specializes in creating transcripts of court proceedings. Other legal professionals, such as lawyers and judges, may rely on court reporters to create accurate records of what was said during a court case. There are a number of ways that court reporters can utilize legal transcription services. First, court reporters can use transcription services to create transcripts of court proceedings. This can be useful for creating a record of what was said during a court case, or for creating a transcript for appeal purposes. Additionally, court reporters can use transcription services to create transcripts of depositions. This can be helpful for creating a record of what was said during a deposition, or for creating a transcript for use in future court proceedings.</t>
+          <t>A court reporter is an official who uses shorthand or other methods to transcribe judicial proceedings. A court reporter is different from other legal professionals because they are specifically trained to take down verbatim transcriptions of court proceedings. This means that they have to be able to type extremely quickly and accurately in order to keep up with the proceedings. Court reporters also often have to be able to create audio or video recordings of proceedings in addition to taking down the transcripts. There are many ways that court reporters can utilize legal transcription services. They can use them to transcribe witness testimony, court proceedings, and deposition transcripts.</t>
         </is>
       </c>
       <c r="AS3" t="inlineStr">
         <is>
-          <t>Legal transcription services can be a valuable resource for court reporters. Court reporters are legal professionals who specialize in creating transcripts of court proceedings. They use a special type of shorthand to take down verbatim transcripts of what is said in court, which can be used as evidence in legal proceedings. Transcription services can provide court reporters with an efficient and accurate way to transcribe court proceedings and depositions.
-At Capital Typing, we provide legal transcription services for court reporters. Our services are designed to help court reporters create accurate records of court proceedings and depositions. We utilize the latest technology and experienced transcriptionists to ensure that your transcripts are accurate and of the highest quality.
-Our transcription services are tailored to the specific needs of court reporters. We can provide you with transcripts of court proceedings and depositions quickly and efficiently. Our experienced transcriptionists can transcribe in a variety of legal formats, including audio, video, and handwritten documents. We can also produce transcripts in a variety</t>
+          <t>Court reporters are a vital part of the legal system, providing verbatim transcriptions of court proceedings. They require specialized training in order to accurately and quickly take down the words spoken in the courtroom. In addition to transcribing proceedings, court reporters may also be responsible for creating audio or video recordings of proceedings. 
+Given the complexity of their role, court reporters need reliable transcription services to support their work. Capital Typing offers comprehensive legal transcription services for court reporters, allowing them to quickly and accurately transcribe witness testimony, court proceedings, and deposition transcripts.
+Capital Typing provides experienced transcribers who understand the legal system and the unique needs of court reporters. Their transcriptionists are reliable, accurate, and can quickly transcribe documents, allowing court reporters to focus on their primary responsibilities. 
+Capital Typing is committed to providing court reporters with the most accurate and efficient legal transcription services. Their team of transcribers is well-trained and experienced in the legal</t>
         </is>
       </c>
     </row>
@@ -870,8 +889,8 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Services by Smart Transcribe
-As a freelance transcriptionist, I find dealing with multiple projects and clients quite a stressful task. Smart Transcribe have been extremely helpful in reducing this stress within my job. While they are always quick to respond to any of my requests, I have also found that they are extremely good at matching me to transcriptions that are within my range of abilities. As a result, I am very happy with the work that I have done for Smart Transcribe and the relationships I have formed with the company.</t>
+          <t>August 10, 2008 | Hayley Halpin Medical transcription is a time-consuming task and often requires a high degree of expertise. This has led to many businesses using transcription outsourcing as a means of increasing efficiency without increasing costs. The doctors, interviewers, or other speakers mail or e-mail their audio files to the transcriptionist, who then transcribes them into a word… Continue Reading →
+It Real</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -881,11 +900,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>There are quite a few reasons why some businesses choose to outsource transcription services. The savings in terms of both time and money is significant. Here we will explore some of the many benefits of outsourcing transcription services.
-The benefit of savings in terms of time is that businesses can redirect their energies to other tasks that invaluable. The time savings can really add up and help a business to get back on track.
-Another huge benefit of outsourcing transcription services is the reduction in turnover rates. With the increased accuracy that transcription services provide, businesses can keep better track of their turnover rates. This means that businesses can make more money and keep their customers happy.
-Transcription services can provide a wide variety of benefits. These benefits can be discovered by exploring the different types of services that outsourcing provides. With the increased accuracy that outsourcing provides, businesses can get back on track and improve their bottom line.
-Outsourcing can save businesses time and money and help to improve the overall quality</t>
+          <t>to save money
+There are many benefits of outsourcing transcription services if you are looking to reduce your overall costs. This type of service can save you both time and money, and it can also provide you with a higher quality finished product. Below is a look at some of the main benefits of outsourcing your needs:
+1. Save time
+One of the biggest advantages of outsourcing transcription services is that it can save you a lot of time. This type of service can be used for a variety of tasks, including recording telephone calls, meetings, interviews, and more. Rather than transcribing these files yourself, you can simply send them to a service provider who will handle the task for you.
+2. Save money
+In addition to saving time, outsourcing transcription services can also save you money. This type of service can be very affordable, especially when compared to the cost of hiring an in-house transcriptionist. In many cases, you can even find services that offer discounts</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -896,9 +916,8 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>Services
-A recent survey has found that the larger majority of employees working in corporate circles have a preference for working for companies that outsource transcription services. This means that companies are very interested in maintaining a successful image in the eyes of their employees. Therefore, compared to other companies that still hold onto their internalized transcription services, those that outsource transcription services are considered a better bet for career advancement.
-As a fertilizer for career growth, corporate transcription services are very useful. A recent study showed that compelling speech at conferences is two to three times more effective at getting ideas across than written messages. This means that corporate transcription services can help increase knowledge retention and boost effective communication in the workplace. Since successful communication is primary to effective learning, the impact of corporate transcription services is evident.
-Written transcription services have specific purposes and benefits. TheyLondon Private investigators can be used to record business meetings, transcribe speeches and yearly reports, and transcribe lectures. The availability of transcription services will make</t>
+If you work in a medical listening and transcription field, you're already aware of the importance ofaccuratera interpreting services visceral. Researchers have various ways of missile digital media Transcripts – themost popular wayis to transcribe an audio or video into text form using the machine. However, it does not capturesall the necessary information. Hence, transcription companies are embracing technology to advance their workflow.
+For every business, technological advances can influence the aspects of its processes so it is important to achievinga greater success in a short period of time. Nowadays, many audio transcription companies outsourcing transcription services are relying on different types of sophisticated technical equipment to transcription the service they provide. Moore's Lawpredicts that "processing power doubles in capacity and halves in price every 18 months". When applied in a dizzying variety of ways, it can be reviewed previrusesthat hardware prices have indeed dropped significantly over the recent years, meaning that advanced technical equipment is now more accessibility and produces better</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -908,17 +927,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Services
-When you outsource transcription services to a third-party provider, you are relying on that provider to keep your information confidential. The transcription services company should have implementing security measures to protect your confidential information. The security measures might include the following:
-All employees are required to sign confidentiality agreements.
-All employees undergo criminal background checks prior to being hired.
-All employees are trained to handle and protect confidential information.
-Security as an employee is allowed access to a specific transcription services job.
-Recorded phone calls/conversations are protected per confidentiality agreement.
-Paper copies of transcripts are transmitted using physical securityring mail only.
-Auditing procedures in place to help ensure data security.
-Data management procedures and secure document sharing when you outsource transcription services.
-Transcription services companies use secure file sharing/transmission services and have strict rules about how files are to be transmitted (two-factor authentication, encryption, etc.).</t>
+          <t>When outsourcing transcription to a company, you should always consider the security of your data and information. Make sure you understand what type of security the company has in place and what type of access they have to your data. You should also consider the type of data you are outsourcing and whether or not it is confidential or private.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -966,33 +975,23 @@
       </c>
       <c r="AR4" t="inlineStr">
         <is>
-          <t>Services by Smart Transcribe
-As a freelance transcriptionist, I find dealing with multiple projects and clients quite a stressful task. Smart Transcribe have been extremely helpful in reducing this stress within my job. While they are always quick to respond to any of my requests, I have also found that they are extremely good at matching me to transcriptions that are within my range of abilities. As a result, I am very happy with the work that I have done for Smart Transcribe and the relationships I have formed with the company. There are quite a few reasons why some businesses choose to outsource transcription services. The savings in terms of both time and money is significant. Here we will explore some of the many benefits of outsourcing transcription services.
-The benefit of savings in terms of time is that businesses can redirect their energies to other tasks that invaluable. The time savings can really add up and help a business to get back on track.
-Another huge benefit of outsourcing transcription services is the reduction in turnover rates. With the increased accuracy that transcription services provide, businesses can keep better track of their turnover rates. This means that businesses can make more money and keep their customers happy.
-Transcription services can provide a wide variety of benefits. These benefits can be discovered by exploring the different types of services that outsourcing provides. With the increased accuracy that outsourcing provides, businesses can get back on track and improve their bottom line.
-Outsourcing can save businesses time and money and help to improve the overall quality Services
-A recent survey has found that the larger majority of employees working in corporate circles have a preference for working for companies that outsource transcription services. This means that companies are very interested in maintaining a successful image in the eyes of their employees. Therefore, compared to other companies that still hold onto their internalized transcription services, those that outsource transcription services are considered a better bet for career advancement.
-As a fertilizer for career growth, corporate transcription services are very useful. A recent study showed that compelling speech at conferences is two to three times more effective at getting ideas across than written messages. This means that corporate transcription services can help increase knowledge retention and boost effective communication in the workplace. Since successful communication is primary to effective learning, the impact of corporate transcription services is evident.
-Written transcription services have specific purposes and benefits. TheyLondon Private investigators can be used to record business meetings, transcribe speeches and yearly reports, and transcribe lectures. The availability of transcription services will make Services
-When you outsource transcription services to a third-party provider, you are relying on that provider to keep your information confidential. The transcription services company should have implementing security measures to protect your confidential information. The security measures might include the following:
-All employees are required to sign confidentiality agreements.
-All employees undergo criminal background checks prior to being hired.
-All employees are trained to handle and protect confidential information.
-Security as an employee is allowed access to a specific transcription services job.
-Recorded phone calls/conversations are protected per confidentiality agreement.
-Paper copies of transcripts are transmitted using physical securityring mail only.
-Auditing procedures in place to help ensure data security.
-Data management procedures and secure document sharing when you outsource transcription services.
-Transcription services companies use secure file sharing/transmission services and have strict rules about how files are to be transmitted (two-factor authentication, encryption, etc.).</t>
+          <t>August 10, 2008 | Hayley Halpin Medical transcription is a time-consuming task and often requires a high degree of expertise. This has led to many businesses using transcription outsourcing as a means of increasing efficiency without increasing costs. The doctors, interviewers, or other speakers mail or e-mail their audio files to the transcriptionist, who then transcribes them into a word… Continue Reading →
+It Real to save money
+There are many benefits of outsourcing transcription services if you are looking to reduce your overall costs. This type of service can save you both time and money, and it can also provide you with a higher quality finished product. Below is a look at some of the main benefits of outsourcing your needs:
+1. Save time
+One of the biggest advantages of outsourcing transcription services is that it can save you a lot of time. This type of service can be used for a variety of tasks, including recording telephone calls, meetings, interviews, and more. Rather than transcribing these files yourself, you can simply send them to a service provider who will handle the task for you.
+2. Save money
+In addition to saving time, outsourcing transcription services can also save you money. This type of service can be very affordable, especially when compared to the cost of hiring an in-house transcriptionist. In many cases, you can even find services that offer discounts Services
+If you work in a medical listening and transcription field, you're already aware of the importance ofaccuratera interpreting services visceral. Researchers have various ways of missile digital media Transcripts – themost popular wayis to transcribe an audio or video into text form using the machine. However, it does not capturesall the necessary information. Hence, transcription companies are embracing technology to advance their workflow.
+For every business, technological advances can influence the aspects of its processes so it is important to achievinga greater success in a short period of time. Nowadays, many audio transcription companies outsourcing transcription services are relying on different types of sophisticated technical equipment to transcription the service they provide. Moore's Lawpredicts that "processing power doubles in capacity and halves in price every 18 months". When applied in a dizzying variety of ways, it can be reviewed previrusesthat hardware prices have indeed dropped significantly over the recent years, meaning that advanced technical equipment is now more accessibility and produces better When outsourcing transcription to a company, you should always consider the security of your data and information. Make sure you understand what type of security the company has in place and what type of access they have to your data. You should also consider the type of data you are outsourcing and whether or not it is confidential or private.</t>
         </is>
       </c>
       <c r="AS4" t="inlineStr">
         <is>
-          <t>Businesses have found that outsourcing transcription services can save them both time and money. In addition to saving money, transcription services help to reduce turnover rates and promote better communication in the workplace. When done properly, outsourcing transcription services can provide a variety of benefits.
-One of the biggest benefits of outsourcing transcription services is the time savings that it can provide. When businesses outsource transcription services, they can redirect their energies to other tasks that are invaluable. This time savings can really add up and help a business to get back on track.
-Another benefit of outsourcing transcription services is the reduction in turnover rates. With the increased accuracy that transcription services provide, businesses can keep better track of their turnover rates. This means that businesses can make more money and keep their customers happy.
-In addition to the financial benefits that transcription services can provide, they can also help to improve the overall quality of communication in the workplace. A recent survey has found that the larger majority of employees working in corporate</t>
+          <t>Outsourcing transcription services can be a great way to save time and money for any business. It can be used for a variety of tasks such as recording phone calls, meetings, interviews, and more. By outsourcing these services, businesses can access a higher quality finished product without having to spend time and resources on transcribing the files themselves.
+The first benefit of outsourcing transcription services is that it can save time. This type of service is incredibly efficient and can be used to quickly and accurately transcribe audio files into text. By outsourcing this service, businesses can save time and energy that would otherwise be spent on transcribing the files themselves.
+In addition to saving time, outsourcing transcription services can also save money. It is often much more affordable than hiring an in-house transcriptionist, and many services also offer discounts. This can be a great way to cut costs without sacrificing quality.
+Another benefit of outsourcing transcription services is that it can provide businesses with a higher quality</t>
         </is>
       </c>
     </row>

</xml_diff>